<commit_message>
add period test for rs_me
</commit_message>
<xml_diff>
--- a/backtest/rotation_strategy/bt_report/rs_me_ind/single_run/summary.xlsx
+++ b/backtest/rotation_strategy/bt_report/rs_me_ind/single_run/summary.xlsx
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>63422951.81110947</v>
+        <v>69275208.60878387</v>
       </c>
       <c r="C8" s="13" t="n"/>
       <c r="D8" s="13" t="n"/>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>8549.23700946942</v>
+        <v>7359.605883870274</v>
       </c>
       <c r="C9" s="13" t="n"/>
       <c r="D9" s="13" t="n"/>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>5.342295181110947</v>
+        <v>5.927520860878387</v>
       </c>
       <c r="C10" s="13" t="n"/>
       <c r="D10" s="13" t="n"/>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>0.2620688647520155</v>
+        <v>0.2761825681076635</v>
       </c>
       <c r="C11" s="13" t="n"/>
       <c r="D11" s="13" t="n"/>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>6.342295181110947</v>
+        <v>6.927520860878387</v>
       </c>
       <c r="C12" s="13" t="n"/>
       <c r="D12" s="13" t="n"/>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>116.6958276517722</v>
+        <v>132.5283336252121</v>
       </c>
       <c r="C14" s="13" t="n"/>
       <c r="D14" s="13" t="n"/>
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>0.3783371976311861</v>
+        <v>0.4234118907861719</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>0.2290160762715983</v>
+        <v>0.232873654013217</v>
       </c>
       <c r="C16" s="13" t="n"/>
       <c r="D16" s="13" t="n"/>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>0.943447061794546</v>
+        <v>0.9794222022626694</v>
       </c>
       <c r="C17" s="13" t="n"/>
       <c r="D17" s="13" t="n"/>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>0.1611293772800286</v>
+        <v>0.1636922851084789</v>
       </c>
       <c r="C18" s="13" t="n"/>
       <c r="D18" s="13" t="n"/>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1.340938244220071</v>
+        <v>1.393355996658182</v>
       </c>
       <c r="C19" s="13" t="n"/>
       <c r="D19" s="13" t="n"/>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>0.2316823715795179</v>
+        <v>0.2178050998088338</v>
       </c>
       <c r="C20" s="13" t="n"/>
       <c r="D20" s="13" t="n"/>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>0.02307590759201929</v>
+        <v>0.02343572250189203</v>
       </c>
       <c r="C21" s="13" t="n"/>
       <c r="D21" s="13" t="n"/>
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="B22" s="7" t="n">
-        <v>0.968011751550803</v>
+        <v>1.174402049485087</v>
       </c>
       <c r="C22" s="13" t="n"/>
       <c r="D22" s="13" t="n"/>
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="B23" s="7" t="n">
-        <v>0.08904917061459416</v>
+        <v>0.102820475778709</v>
       </c>
       <c r="C23" s="13" t="n"/>
       <c r="D23" s="13" t="n"/>
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B24" s="7" t="n">
-        <v>0.1977936742876501</v>
+        <v>0.2111939341669929</v>
       </c>
       <c r="C24" s="13" t="n"/>
       <c r="D24" s="13" t="n"/>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="B25" s="7" t="n">
-        <v>0.4111300937602889</v>
+        <v>0.4255720106798229</v>
       </c>
       <c r="C25" s="13" t="n"/>
       <c r="D25" s="13" t="n"/>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B26" s="7" t="n">
-        <v>1.18315521215723</v>
+        <v>1.240522827588527</v>
       </c>
       <c r="C26" s="13" t="n"/>
       <c r="D26" s="13" t="n"/>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B27" s="7" t="n">
-        <v>0.4540542961486568</v>
+        <v>0.5033413103061697</v>
       </c>
       <c r="C27" s="13" t="n"/>
       <c r="D27" s="13" t="n"/>
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="B28" s="7" t="n">
-        <v>0.5914549555405634</v>
+        <v>0.5752545670093641</v>
       </c>
       <c r="C28" s="13" t="n"/>
       <c r="D28" s="13" t="n"/>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B29" s="7" t="n">
-        <v>0.2646041508229348</v>
+        <v>0.2625688207072752</v>
       </c>
       <c r="C29" s="13" t="n"/>
       <c r="D29" s="13" t="n"/>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>0.1908184015450558</v>
+        <v>0.2038540411549403</v>
       </c>
       <c r="C30" s="13" t="n"/>
       <c r="D30" s="13" t="n"/>
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>0.4407723715238324</v>
+        <v>0.4554737246943359</v>
       </c>
       <c r="C31" s="13" t="n"/>
       <c r="D31" s="13" t="n"/>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>0.9237617112274074</v>
+        <v>0.9606978695064294</v>
       </c>
       <c r="C32" s="13" t="n"/>
       <c r="D32" s="13" t="n"/>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>1.445168761394323</v>
+        <v>1.506285351860959</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>1.1578970794012</v>
+        <v>1.217863871985986</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>0.03465837362030417</v>
+        <v>0.03436096729415219</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="B36" s="16" t="n">
-        <v>0.2095995585019905</v>
+        <v>0.2064661979200169</v>
       </c>
     </row>
   </sheetData>
@@ -1157,16 +1157,16 @@
         <v>2014</v>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0.9037669999999998</v>
+        <v>0.9554459999999979</v>
       </c>
       <c r="C2" s="13" t="n">
-        <v>0.7362378392252324</v>
+        <v>0.7833732082589765</v>
       </c>
       <c r="D2" s="13" t="n">
-        <v>3.360872885684619</v>
+        <v>3.477933820119619</v>
       </c>
       <c r="E2" s="13" t="n">
-        <v>5.711919635221625</v>
+        <v>6.044945150177945</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>0.6052631578947368</v>
@@ -1177,16 +1177,16 @@
         <v>2015</v>
       </c>
       <c r="B3" s="13" t="n">
-        <v>1.104497556686297</v>
+        <v>1.156042150997778</v>
       </c>
       <c r="C3" s="13" t="n">
-        <v>-0.01371054542823455</v>
+        <v>0.0137412672060071</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>2.529103193819449</v>
+        <v>2.580546725723143</v>
       </c>
       <c r="E3" s="13" t="n">
-        <v>3.179394975289946</v>
+        <v>3.360584824538321</v>
       </c>
       <c r="F3" s="13" t="n">
         <v>0.4423076923076923</v>
@@ -1197,16 +1197,16 @@
         <v>2016</v>
       </c>
       <c r="B4" s="13" t="n">
-        <v>-0.1198503022483871</v>
+        <v>-0.07852730439864536</v>
       </c>
       <c r="C4" s="13" t="n">
-        <v>0.121305566443253</v>
+        <v>0.1757124455867206</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>-0.6448375505647599</v>
+        <v>-0.3608811647581712</v>
       </c>
       <c r="E4" s="13" t="n">
-        <v>-0.3101626196347356</v>
+        <v>-0.01044731754874058</v>
       </c>
       <c r="F4" s="13" t="n">
         <v>0.5600000000000001</v>
@@ -1217,16 +1217,16 @@
         <v>2017</v>
       </c>
       <c r="B5" s="13" t="n">
-        <v>0.2759501754815812</v>
+        <v>0.2555867500001928</v>
       </c>
       <c r="C5" s="13" t="n">
-        <v>0.404708586227513</v>
+        <v>0.3825494957883834</v>
       </c>
       <c r="D5" s="13" t="n">
-        <v>1.735219249924616</v>
+        <v>1.605037259941543</v>
       </c>
       <c r="E5" s="13" t="n">
-        <v>2.361555694805246</v>
+        <v>2.18481302088263</v>
       </c>
       <c r="F5" s="13" t="n">
         <v>0.6470588235294118</v>
@@ -1237,19 +1237,19 @@
         <v>2018</v>
       </c>
       <c r="B6" s="13" t="n">
-        <v>-0.08047956850924734</v>
+        <v>-0.07101160275553356</v>
       </c>
       <c r="C6" s="13" t="n">
-        <v>0.2188131265219364</v>
+        <v>0.231630843534265</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>-0.4424803177135904</v>
+        <v>-0.375356396202483</v>
       </c>
       <c r="E6" s="13" t="n">
-        <v>-0.04000728111666108</v>
+        <v>0.03183147327606684</v>
       </c>
       <c r="F6" s="13" t="n">
-        <v>0.5882352941176471</v>
+        <v>0.6078431372549019</v>
       </c>
     </row>
     <row r="7">
@@ -1257,19 +1257,19 @@
         <v>2019</v>
       </c>
       <c r="B7" s="13" t="n">
-        <v>0.3402214503766974</v>
+        <v>0.3650715678187341</v>
       </c>
       <c r="C7" s="13" t="n">
-        <v>-0.09222181213630309</v>
+        <v>-0.07465448084793611</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>1.447730480768292</v>
+        <v>1.514539092802319</v>
       </c>
       <c r="E7" s="13" t="n">
-        <v>0.4818632600685998</v>
+        <v>0.6042028596796424</v>
       </c>
       <c r="F7" s="13" t="n">
-        <v>0.3461538461538461</v>
+        <v>0.3846153846153846</v>
       </c>
     </row>
     <row r="8">
@@ -1277,19 +1277,19 @@
         <v>2020</v>
       </c>
       <c r="B8" s="13" t="n">
-        <v>0.2018984074975415</v>
+        <v>0.1484274543593994</v>
       </c>
       <c r="C8" s="13" t="n">
-        <v>-0.29470664865673</v>
+        <v>-0.3254053518943449</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>0.8468640560927785</v>
+        <v>0.6678824442099208</v>
       </c>
       <c r="E8" s="13" t="n">
-        <v>-1.350746858978936</v>
+        <v>-1.729473658497802</v>
       </c>
       <c r="F8" s="13" t="n">
-        <v>0.4038461538461539</v>
+        <v>0.3846153846153846</v>
       </c>
     </row>
     <row r="9">
@@ -1297,19 +1297,19 @@
         <v>2021</v>
       </c>
       <c r="B9" s="13" t="n">
-        <v>-0.09445818920838037</v>
+        <v>-0.05627889842548772</v>
       </c>
       <c r="C9" s="13" t="n">
-        <v>-0.2223936280737484</v>
+        <v>-0.1879518526650552</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>-0.3301401486741506</v>
+        <v>-0.1354596536649402</v>
       </c>
       <c r="E9" s="13" t="n">
-        <v>-0.8338588014762628</v>
+        <v>-0.6368453856414227</v>
       </c>
       <c r="F9" s="13" t="n">
-        <v>0.4615384615384616</v>
+        <v>0.4807692307692308</v>
       </c>
     </row>
     <row r="10">
@@ -1317,19 +1317,19 @@
         <v>2022</v>
       </c>
       <c r="B10" s="13" t="n">
-        <v>0.05094440577094433</v>
+        <v>0.03331477275422322</v>
       </c>
       <c r="C10" s="13" t="n">
-        <v>0.202423207723403</v>
+        <v>0.1851668263673923</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>0.8782359440944111</v>
+        <v>0.5370925200657047</v>
       </c>
       <c r="E10" s="13" t="n">
-        <v>1.228039773106829</v>
+        <v>0.9152616411622262</v>
       </c>
       <c r="F10" s="13" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.52</v>
       </c>
     </row>
   </sheetData>
@@ -1436,28 +1436,28 @@
         <v>-0.04519900000000021</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>0.01017175306686946</v>
+        <v>0.01787702358920873</v>
       </c>
       <c r="G2" s="15" t="n">
-        <v>0.02473372572479593</v>
+        <v>0.02471729758095154</v>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.05950510386303076</v>
+        <v>0.06830559940234537</v>
       </c>
       <c r="I2" s="15" t="n">
-        <v>0.005179615386819103</v>
+        <v>0.005229731266630511</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>0.06280602618643716</v>
+        <v>0.06254809575859599</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>0.02528076830938342</v>
+        <v>0.02551974480255237</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.2217196542626929</v>
+        <v>0.2361729057170436</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.3585623452341027</v>
+        <v>0.357378323690394</v>
       </c>
     </row>
     <row r="3">
@@ -1465,40 +1465,40 @@
         <v>2015</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>-0.02881865270277295</v>
+        <v>-0.01568491280250217</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>0.1187239135855154</v>
+        <v>0.133934096193062</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>0.1944733447688374</v>
+        <v>0.1842494712650418</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>0.199440797874902</v>
+        <v>0.2075157513139803</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>0.2231898749212902</v>
+        <v>0.2079509860714526</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>-0.04383695953838218</v>
+        <v>-0.0417627958076463</v>
       </c>
       <c r="H3" s="15" t="n">
         <v>0</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.03335913699029702</v>
+        <v>0.01979349242606276</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>0</v>
+        <v>-0.004997069887591854</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>0.08517879335045242</v>
+        <v>0.1197899801650353</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>0.05964686945531983</v>
+        <v>0.05858944585076897</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>-0.02718486064599357</v>
+        <v>-0.0297666183163644</v>
       </c>
     </row>
     <row r="4">
@@ -1506,40 +1506,40 @@
         <v>2016</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>-0.08409166865719542</v>
+        <v>-0.08406308882492131</v>
       </c>
       <c r="C4" s="15" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>0.03832828005086175</v>
+        <v>0.06015674283174999</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>-0.0378215373955767</v>
+        <v>-0.03778218106193698</v>
       </c>
       <c r="F4" s="15" t="n">
-        <v>0</v>
+        <v>0.01412481655711506</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>0.01731430276626278</v>
+        <v>0.01522349368366216</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>-0.0133618334299489</v>
+        <v>-0.01337921450681401</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>-0.001059312821761749</v>
+        <v>-0.0005320595226910863</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>-0.02878929095506166</v>
+        <v>-0.0287987681853562</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>-0.001214558681867706</v>
+        <v>-0.01131708326811054</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>0.01362991963675997</v>
+        <v>0.03672206263731503</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>-0.02434478741991863</v>
+        <v>-0.02417342553357116</v>
       </c>
     </row>
     <row r="5">
@@ -1547,40 +1547,40 @@
         <v>2017</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>-0.0001599411960878649</v>
+        <v>0.001221122222648363</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>0.03071730919990512</v>
+        <v>0.03067027106238407</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.009416260116515529</v>
+        <v>0.009567739330051506</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.01518243566690636</v>
+        <v>0.01507875523490676</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>-0.002902835568194484</v>
+        <v>-0.005441805636724584</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>0.063624403637357</v>
+        <v>0.07386646474247982</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.03733217939722699</v>
+        <v>0.03220649239421092</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>0.03272611440092499</v>
+        <v>0.03295954061228601</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>0.005071978894290119</v>
+        <v>0.005088450461457672</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>0.05544790271360411</v>
+        <v>0.0557391322100691</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>-0.01485627886499064</v>
+        <v>-0.01482572819807237</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>0.01762291587460174</v>
+        <v>-0.002627412644663485</v>
       </c>
     </row>
     <row r="6">
@@ -1588,28 +1588,28 @@
         <v>2018</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.03610054545317176</v>
+        <v>0.03609099256584747</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.05926048434427156</v>
+        <v>-0.05926563052477252</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>0.01304968342603541</v>
+        <v>0.0253591608306889</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>-0.02446487861083324</v>
+        <v>-0.02441977245463778</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.07539930573581355</v>
+        <v>0.07586284766538154</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>-0.04694336167137847</v>
+        <v>-0.04697427286178646</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>-0.04510819830822299</v>
+        <v>-0.04150249098614511</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>-0.03384137637235618</v>
+        <v>-0.0339088575096278</v>
       </c>
       <c r="J6" s="15" t="n">
         <v>0</v>
@@ -1618,10 +1618,10 @@
         <v>0</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>-0.01803274448312842</v>
+        <v>-0.02789917417966115</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>0.02808345892593755</v>
+        <v>0.0323440021268786</v>
       </c>
     </row>
     <row r="7">
@@ -1629,40 +1629,40 @@
         <v>2019</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>-0.03093319991201904</v>
+        <v>-0.02987549834425918</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>0.294535866815355</v>
+        <v>0.2945114163041314</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>0.04889838889701359</v>
+        <v>0.0491441149047751</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>-0.00136261053989728</v>
+        <v>-0.02339651336025994</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>-0.0188743069126267</v>
+        <v>-0.01833705608271641</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>-0.01169493505074026</v>
+        <v>0.009498949666450152</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>-0.02913961028182777</v>
+        <v>-0.03283631580195201</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>0.02299615743984607</v>
+        <v>0.02143336440888755</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>0.02171255253660687</v>
+        <v>0.02189229003114956</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>0.009473177308342962</v>
+        <v>0.009347744210417508</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>-0.03837730039820475</v>
+        <v>-0.02828064846554923</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>0.06780720511975158</v>
+        <v>0.08119384139537589</v>
       </c>
     </row>
     <row r="8">
@@ -1670,40 +1670,40 @@
         <v>2020</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>0.04446768519590605</v>
+        <v>0.0446181029869881</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>-0.08117673974885276</v>
+        <v>-0.08589811245421153</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>-0.07841679921583056</v>
+        <v>-0.07845301603871235</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>0.01612616758873409</v>
+        <v>0.006788078040668388</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.03207180269310261</v>
+        <v>0.03207478691469778</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>0.1283512839114451</v>
+        <v>0.1283950752612617</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.1850020429028558</v>
+        <v>0.185002864165839</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>-0.02961352775730175</v>
+        <v>-0.04842882336747911</v>
       </c>
       <c r="J8" s="15" t="n">
-        <v>-0.07124917971025391</v>
+        <v>-0.07125095250825797</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.01566759526615957</v>
+        <v>-0.02813849769823817</v>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.05074794214482514</v>
+        <v>0.05079440486753906</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>0.03968306960949119</v>
+        <v>0.04074018783487454</v>
       </c>
     </row>
     <row r="9">
@@ -1711,40 +1711,40 @@
         <v>2021</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>0.02404268319399461</v>
+        <v>0.02405187967247069</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>-0.09582487433301801</v>
+        <v>-0.08893335263272439</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>-0.03596445738029552</v>
+        <v>-0.03565582582023019</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>0.008478495374700579</v>
+        <v>0.003148535494480242</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>0.02939524761328061</v>
+        <v>0.02946675178233726</v>
       </c>
       <c r="G9" s="15" t="n">
-        <v>-0.02295287539638635</v>
+        <v>-0.02293367964539028</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>0.03959405568757246</v>
+        <v>0.05625236656452492</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.01747654972376833</v>
+        <v>0.03494330451265037</v>
       </c>
       <c r="J9" s="15" t="n">
-        <v>-0.07749968741470503</v>
+        <v>-0.07434255692166258</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>-0.001896856717510276</v>
+        <v>-0.001142367316066539</v>
       </c>
       <c r="L9" s="15" t="n">
-        <v>-3.505507645995554e-05</v>
+        <v>0.00188970811695377</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.02698859019366151</v>
+        <v>0.02654933518711711</v>
       </c>
     </row>
     <row r="10">
@@ -1752,25 +1752,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>-0.04690669350189636</v>
+        <v>-0.04643331847194276</v>
       </c>
       <c r="C10" s="15" t="n">
-        <v>0</v>
+        <v>0.01331951378378049</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0</v>
+        <v>-0.04969245260824828</v>
       </c>
       <c r="E10" s="15" t="n">
-        <v>0</v>
+        <v>0.004584058425140647</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>-0.0001599505405111001</v>
+        <v>0.01600397908458073</v>
       </c>
       <c r="G10" s="15" t="n">
-        <v>0.09495296180152635</v>
+        <v>0.09478871887767415</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.007206063790879291</v>
+        <v>0.007068428693084217</v>
       </c>
       <c r="I10" s="15" t="n">
         <v/>
@@ -1892,28 +1892,28 @@
         <v>0.01842302582723909</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>-0.02103303812915192</v>
+        <v>-0.01354014655508384</v>
       </c>
       <c r="G2" s="15" t="n">
-        <v>-0.03903597901584033</v>
+        <v>-0.03905146802687398</v>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.1051005186003746</v>
+        <v>0.114228123583185</v>
       </c>
       <c r="I2" s="15" t="n">
-        <v>-0.05305635315682089</v>
+        <v>-0.05301254954620394</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>-0.01783728006402474</v>
+        <v>-0.01807968525303372</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>0.04373530700889217</v>
+        <v>0.04397591613464469</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.1736451047486089</v>
+        <v>0.1875533542419348</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.4393596187610667</v>
+        <v>0.4381238533848337</v>
       </c>
     </row>
     <row r="3">
@@ -1921,40 +1921,40 @@
         <v>2015</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>-0.1570484809948258</v>
+        <v>-0.1449884808776242</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>-0.02521553171746027</v>
+        <v>-0.01168937799534742</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>-0.01473645638524501</v>
+        <v>-0.02325502154919745</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>-0.0208067362330786</v>
+        <v>-0.01416353362077638</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>-0.01448602490666651</v>
+        <v>-0.02687217179248036</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>0.1573927578098213</v>
+        <v>0.1600036826378639</v>
       </c>
       <c r="H3" s="15" t="n">
         <v>0.08807385286485769</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.2672544097838581</v>
+        <v>0.2507615094025863</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>-0.06960194198380509</v>
+        <v>-0.0742157423819666</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>-0.09365381410225404</v>
+        <v>-0.06272146575269288</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>-0.01844589474933678</v>
+        <v>-0.01946159371676992</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>-0.04428263436760183</v>
+        <v>-0.04682988404664079</v>
       </c>
     </row>
     <row r="4">
@@ -1962,40 +1962,40 @@
         <v>2016</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>0.2059736006216251</v>
+        <v>0.2060083814052398</v>
       </c>
       <c r="C4" s="15" t="n">
         <v>0.04481461253681185</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>-0.1367187974345919</v>
+        <v>-0.1180637126000554</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>0.00319031772590761</v>
+        <v>0.00323135719180212</v>
       </c>
       <c r="F4" s="15" t="n">
-        <v>-0.01869687499886785</v>
+        <v>-0.004003420854947537</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>-0.01571172317230574</v>
+        <v>-0.01773117161335924</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>0.034753783185413</v>
+        <v>0.03473555427032005</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>-0.03448025951692668</v>
+        <v>-0.03397063994347815</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>-0.01094468200686183</v>
+        <v>-0.01095421805216723</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>-0.00714708096038652</v>
+        <v>-0.01703532580380018</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>0.001991342098054405</v>
+        <v>0.02475251472445716</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>0.0822265384303229</v>
+        <v>0.08241059865140365</v>
       </c>
     </row>
     <row r="5">
@@ -2003,40 +2003,40 @@
         <v>2017</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>0.03668880282065068</v>
+        <v>0.03813329109922958</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>0.008549856544281864</v>
+        <v>0.008503285688379103</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.01920326083335477</v>
+        <v>0.01935533915928955</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.04507756959205866</v>
+        <v>0.04496975905270451</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>0.0443653844641656</v>
+        <v>0.04170589570949557</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>0.03056273252904584</v>
+        <v>0.04051432393793242</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.08184425312448762</v>
+        <v>0.07648953218758381</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>-0.03067675236856549</v>
+        <v>-0.03045383247100908</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>-0.003950205800136053</v>
+        <v>-0.003929186784302985</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>0.05245864705801195</v>
+        <v>0.05274402532707301</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>0.03928684245551106</v>
+        <v>0.03932080026702889</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>0.02576844085693675</v>
+        <v>0.005510982861347546</v>
       </c>
     </row>
     <row r="6">
@@ -2044,28 +2044,28 @@
         <v>2018</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.04345253582373698</v>
+        <v>0.04344309384720302</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.07486758233001567</v>
+        <v>-0.07487212070987559</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>-0.06888372990124181</v>
+        <v>-0.05739992670256899</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>0.02307722640475873</v>
+        <v>0.02312375297689684</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.1115065135515318</v>
+        <v>0.1119865071413886</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>0.02878913902575575</v>
+        <v>0.02875466938355076</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>-0.02132634247483933</v>
+        <v>-0.01762543413900142</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>0.04369284823056874</v>
+        <v>0.04362132086580517</v>
       </c>
       <c r="J6" s="15" t="n">
         <v>0.01408128749632898</v>
@@ -2074,10 +2074,10 @@
         <v>0.09307593245600398</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>-0.06101202974392628</v>
+        <v>-0.07040841729180636</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>0.09022484116648233</v>
+        <v>0.09473173631281639</v>
       </c>
     </row>
     <row r="7">
@@ -2085,40 +2085,40 @@
         <v>2019</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>-0.01533640104992007</v>
+        <v>-0.01425782587185154</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>0.03749289115756893</v>
+        <v>0.03746565053886086</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>-0.05029861143010428</v>
+        <v>-0.05006929967698492</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>0.03948868182210918</v>
+        <v>0.01685066495061127</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>0.06231769208254812</v>
+        <v>0.0628260394151039</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>-0.03394623483520987</v>
+        <v>-0.01287323641926952</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>-0.06709589302648888</v>
+        <v>-0.07065816083776022</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>-0.005914080239951547</v>
+        <v>-0.007429002468095969</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>0.01098032244646885</v>
+        <v>0.01117005042157704</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>-0.01859366018351916</v>
+        <v>-0.01871268022507755</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>-0.03515482255718005</v>
+        <v>-0.02492529546418742</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>-0.01205205817117616</v>
+        <v>0.0004313730364355894</v>
       </c>
     </row>
     <row r="8">
@@ -2126,40 +2126,40 @@
         <v>2020</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>-0.0267729046586066</v>
+        <v>-0.02662840480338313</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>-0.1469674148613628</v>
+        <v>-0.1514000709614565</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.01493421424753616</v>
+        <v>0.01489350832691705</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>-0.08517461162432904</v>
+        <v>-0.09355378799316649</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.02252212213655858</v>
+        <v>0.0225256836887997</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>-0.03517510040018101</v>
+        <v>-0.03513719007962413</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.0306187962476987</v>
+        <v>0.03062074297279649</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>-0.009359355425964</v>
+        <v>-0.02773633734745917</v>
       </c>
       <c r="J8" s="15" t="n">
-        <v>-0.01891913156174896</v>
+        <v>-0.01892100260440033</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.049436953899895</v>
+        <v>-0.06133112211940139</v>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.05825666305309452</v>
+        <v>0.05830427858099285</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>-0.07954679718818491</v>
+        <v>-0.07859822819289586</v>
       </c>
     </row>
     <row r="9">
@@ -2167,40 +2167,40 @@
         <v>2021</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>-0.03156115520688685</v>
+        <v>-0.03155103790539338</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>-0.02908303237500931</v>
+        <v>-0.02175794403532316</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0.008329056081903818</v>
+        <v>0.008634592050515089</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>-0.1035439422216831</v>
+        <v>-0.1074742323474593</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>-0.0401792605380934</v>
+        <v>-0.04011213037755468</v>
       </c>
       <c r="G9" s="15" t="n">
-        <v>-0.07257937901139344</v>
+        <v>-0.07256033881386503</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>0.0437847286366464</v>
+        <v>0.06114004260572359</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.0838335288615919</v>
+        <v>0.1031673862071112</v>
       </c>
       <c r="J9" s="15" t="n">
-        <v>-0.08927629008222493</v>
+        <v>-0.08615698976545749</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>-0.03495649521276889</v>
+        <v>-0.0342152042790731</v>
       </c>
       <c r="L9" s="15" t="n">
-        <v>-0.04237862512051849</v>
+        <v>-0.04055603183239676</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.07945978034455448</v>
+        <v>0.0789771067612639</v>
       </c>
     </row>
     <row r="10">
@@ -2208,25 +2208,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>0.08364231794071419</v>
+        <v>0.0841668575969825</v>
       </c>
       <c r="C10" s="15" t="n">
-        <v>0.004280811429914211</v>
+        <v>0.01806208005000176</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.07009750317718355</v>
+        <v>0.01772051533395458</v>
       </c>
       <c r="E10" s="15" t="n">
-        <v>0.1308985363887376</v>
+        <v>0.1371168483904222</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>-0.04059993149316699</v>
+        <v>-0.02471838657143</v>
       </c>
       <c r="G10" s="15" t="n">
-        <v>-0.06464452556788658</v>
+        <v>-0.06478514734454643</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.01740249472517297</v>
+        <v>0.01726485962737789</v>
       </c>
       <c r="I10" s="15" t="n">
         <v/>

</xml_diff>